<commit_message>
Documento historial de versiones
</commit_message>
<xml_diff>
--- a/docs/Historial de Versiones GymBuddy.xlsx
+++ b/docs/Historial de Versiones GymBuddy.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28224"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28318"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ceu365-my.sharepoint.com/personal/daniel_escribanoissacovitch_usp_ceu_es/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1A0F8E7-CC41-4F06-8B9C-0382E67A89D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6741AEFB-7AFE-43D0-873D-D1BBDBFA7571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{C004B29A-B8E5-4DFC-85A2-E773A9387078}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>PLAN DE COMUNICACIONES DE GESTIÓN DEL CAMBIO</t>
   </si>
@@ -117,6 +117,15 @@
   </si>
   <si>
     <t>Entrega de prototipos</t>
+  </si>
+  <si>
+    <t>Entrega de proyecto y documentación</t>
+  </si>
+  <si>
+    <t>Entrega</t>
+  </si>
+  <si>
+    <t>Entrega final y reformulación de documentos</t>
   </si>
   <si>
     <t>fracés si lo lees</t>
@@ -259,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -297,6 +306,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="16" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -309,7 +321,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -647,15 +665,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44E5776-9384-4E98-8CFF-47C5AB8BA00B}">
-  <dimension ref="A1:XFC1048575"/>
+  <dimension ref="A1:XFC1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
     <col min="3" max="3" width="20.28515625" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" customWidth="1"/>
     <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
@@ -665,13 +684,13 @@
   <sheetData>
     <row r="1" spans="1:7" ht="28.5">
       <c r="A1" s="1"/>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:7" ht="25.5" customHeight="1">
       <c r="A2" s="1"/>
@@ -686,10 +705,10 @@
       <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="20"/>
+      <c r="D3" s="23"/>
       <c r="E3" s="11" t="s">
         <v>3</v>
       </c>
@@ -702,15 +721,15 @@
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="20"/>
+      <c r="D4" s="23"/>
       <c r="E4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="19">
-        <v>45604</v>
+      <c r="F4" s="15">
+        <v>45635</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1">
@@ -718,24 +737,24 @@
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="20"/>
+      <c r="D5" s="23"/>
       <c r="E5" s="10" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="16.5" customHeight="1">
       <c r="A6" s="5"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
     </row>
     <row r="7" spans="1:7" ht="37.5">
       <c r="A7" s="5"/>
@@ -758,7 +777,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:7" customFormat="1" ht="25.5">
+    <row r="8" spans="1:7" ht="25.5">
       <c r="A8" s="5"/>
       <c r="B8" s="7" t="s">
         <v>16</v>
@@ -779,7 +798,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:7" customFormat="1" ht="25.5">
+    <row r="9" spans="1:7" ht="25.5">
       <c r="A9" s="5"/>
       <c r="B9" s="7" t="s">
         <v>21</v>
@@ -800,7 +819,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:7" customFormat="1" ht="25.5">
+    <row r="10" spans="1:7" ht="25.5">
       <c r="A10" s="5"/>
       <c r="B10" s="7" t="s">
         <v>24</v>
@@ -821,24 +840,42 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:7" customFormat="1"/>
-    <row r="12" spans="1:7" customFormat="1"/>
-    <row r="16" spans="1:7" customFormat="1" ht="15" customHeight="1"/>
-    <row r="17" customFormat="1" ht="15" customHeight="1"/>
-    <row r="32" customFormat="1" ht="15" customHeight="1"/>
-    <row r="417528" customFormat="1"/>
-    <row r="1048575" spans="16383:16383" customFormat="1">
-      <c r="XFC1048575" s="13" t="s">
+    <row r="11" spans="1:7" ht="37.5">
+      <c r="A11" s="5"/>
+      <c r="B11" s="20" t="s">
         <v>27</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="22">
+        <v>45636</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7"/>
+    <row r="13" spans="1:7"/>
+    <row r="417529"/>
+    <row r="1048576" spans="16383:16383">
+      <c r="XFC1048576" s="13" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="B1:F1"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>